<commit_message>
Versi 1.0.0.22 add ctkHasil.rpt add ctkHasil.vb Cetak Hasil diganti ke CR.
</commit_message>
<xml_diff>
--- a/balailab/ket.xlsx
+++ b/balailab/ket.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="24">
   <si>
     <t>Tabel</t>
   </si>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D24"/>
+  <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="M22" activeCellId="6" sqref="M10 M12 M14 M16 M18 M20 M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -507,9 +507,12 @@
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -523,7 +526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -537,7 +540,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -550,8 +553,32 @@
       <c r="D9" s="2">
         <v>15000</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>15000</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -564,8 +591,32 @@
       <c r="D10" s="2">
         <v>135000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>405000</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10" s="2">
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -578,8 +629,32 @@
       <c r="D11" s="2">
         <v>30000</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>30000</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -592,8 +667,32 @@
       <c r="D12" s="2">
         <v>135000</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>405000</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12" s="2">
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -606,8 +705,32 @@
       <c r="D13" s="2">
         <v>30000</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>30000</v>
+      </c>
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -620,8 +743,32 @@
       <c r="D14" s="2">
         <v>90000</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>270000</v>
+      </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -634,8 +781,32 @@
       <c r="D15" s="2">
         <v>15000</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>15000</v>
+      </c>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -648,8 +819,32 @@
       <c r="D16" s="2">
         <v>45000</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>135000</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -662,8 +857,32 @@
       <c r="D17" s="2">
         <v>7500</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>7500</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -676,8 +895,32 @@
       <c r="D18" s="2">
         <v>45000</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>135000</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -690,8 +933,32 @@
       <c r="D19" s="2">
         <v>7500</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>7500</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -704,8 +971,32 @@
       <c r="D20" s="2">
         <v>90000</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>270000</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20" s="2">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -718,8 +1009,32 @@
       <c r="D21" s="2">
         <v>15000</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>15000</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21" s="2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -732,8 +1047,32 @@
       <c r="D22" s="2">
         <v>45000</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>135000</v>
+      </c>
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -746,10 +1085,50 @@
       <c r="D23" s="2">
         <v>22500</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>22500</v>
+      </c>
+      <c r="K23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23" s="2">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="C24">
+        <f>SUM(C9:C23)</f>
+        <v>64</v>
+      </c>
       <c r="D24" s="2">
         <f>SUM(D9:D23)</f>
+        <v>727500</v>
+      </c>
+      <c r="I24">
+        <f>SUM(I9:I23)</f>
+        <v>1897500</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:N24" si="0">SUM(M9:M23)</f>
+        <v>32</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="0"/>
         <v>727500</v>
       </c>
     </row>

</xml_diff>